<commit_message>
updates kpi41-43 excel defintions
Signed-off-by: anchit-chandran <anchit97123@gmail.com>
</commit_message>
<xml_diff>
--- a/project/npda/dummy_sheets/kpi-specifications/Calculations_AK_20240621 (1).xlsx
+++ b/project/npda/dummy_sheets/kpi-specifications/Calculations_AK_20240621 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ProgrammingWSL\RCPCH\national-paediatric-diabetes-audit\project\npda\dummy_sheets\kpi-specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A25CE-1F74-4850-B751-08B11F0B5E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFAB901-774C-44E4-8330-97221F1F12FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E9E080A3-C8CD-4A00-A462-CC1171CA013C}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="176">
   <si>
     <t>Data Completeness Report Calculations</t>
   </si>
@@ -1020,9 +1020,6 @@
     <t>90 days before or after date of diagnosis</t>
   </si>
   <si>
-    <t>Number of patients with Type 1 diabetes who were diagnosed at least 90 days before the end of the audit period</t>
-  </si>
-  <si>
     <t>4. If diabetes type is inconsistent, we use the most recently reported diabetes type, ordering by visit date.</t>
   </si>
   <si>
@@ -1119,6 +1116,20 @@
   </si>
   <si>
     <t>Number of CYP with T1D aged 12 years and over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of patients with Type 1 diabetes who were diagnosed at least 90 days before the end of the audit period 
+(NOTE: measure 7 AND diabetes diagnosis date &lt; (AUDIT_END_DATE - 90 days))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of patients with Type 1 diabetes who were diagnosed at least 90 days before the end of the audit period  
+(NOTE: measure 7 AND diabetes diagnosis date &lt; (AUDIT_END_DATE - 90 days))
+</t>
+  </si>
+  <si>
+    <t>Number of patients with Type 1 diabetes who were diagnosed at least 14 days before the end of the audit period 
+(NOTE: Measure 7 AND diabetes diagnosis date &lt; (AUDIT_END_DATE - 14 days))</t>
   </si>
 </sst>
 </file>
@@ -1871,17 +1882,17 @@
     </row>
     <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="115.5" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1893,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211B7129-E679-4B7F-BF25-E64EA2BC5452}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -1982,7 +1993,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>26</v>
@@ -2318,7 +2329,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>52</v>
@@ -2335,10 +2346,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>74</v>
@@ -2519,14 +2530,14 @@
         <v>148</v>
       </c>
       <c r="C38" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>165</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>166</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.45">
@@ -2534,13 +2545,13 @@
         <v>32.200000000000003</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>170</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>171</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21"/>
@@ -2550,13 +2561,13 @@
         <v>32.299999999999997</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21"/>
@@ -2715,7 +2726,7 @@
       <c r="E50" s="12"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" ht="105.5" x14ac:dyDescent="0.45">
       <c r="A51" s="13">
         <v>41</v>
       </c>
@@ -2723,7 +2734,7 @@
         <v>112</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>113</v>
@@ -2735,7 +2746,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" ht="105.5" x14ac:dyDescent="0.45">
       <c r="A52" s="13">
         <v>42</v>
       </c>
@@ -2743,7 +2754,7 @@
         <v>115</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>116</v>
@@ -2755,7 +2766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" ht="90.5" x14ac:dyDescent="0.45">
       <c r="A53" s="13">
         <v>43</v>
       </c>
@@ -2763,10 +2774,10 @@
         <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>119</v>
@@ -2832,13 +2843,13 @@
         <v>52</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="F57" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
@@ -2852,13 +2863,13 @@
         <v>52</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E58" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
@@ -2903,62 +2914,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <f0b696580dd64673b338b9e7e9df6a44 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f0b696580dd64673b338b9e7e9df6a44>
-    <Project_x002f__x0020_contract_x0020_end_x0020_date xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195" xsi:nil="true"/>
-    <df98972e859c4d8ab2c40b27a56d4e28 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Research ＆ Quality Improvement</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c788aced-109f-432d-9368-116094370ebc</TermId>
-        </TermInfo>
-      </Terms>
-    </df98972e859c4d8ab2c40b27a56d4e28>
-    <i4add73f68bf4b718053652e70d0f6db xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i4add73f68bf4b718053652e70d0f6db>
-    <l85a7ec099b64d7b82fb97f30e826380 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l85a7ec099b64d7b82fb97f30e826380>
-    <ie61b6fb19f94649bf6a41580239b97e xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Audits</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ae63694e-9999-473c-882e-084b09c6631d</TermId>
-        </TermInfo>
-      </Terms>
-    </ie61b6fb19f94649bf6a41580239b97e>
-    <c7239f321a1b424087383680b3e8c036 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c7239f321a1b424087383680b3e8c036>
-    <bf89ef746e92483cbe19fd955e43c70f xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </bf89ef746e92483cbe19fd955e43c70f>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1be50a68-e751-4212-ab16-e9f1f1e893c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003773CFE9AFA7D54A9CADE54E78DC4341" ma:contentTypeVersion="31" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="661715b63b6f9491f01d170149810120">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="19d55dec-64db-48ca-8a2a-bb7d318d4195" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="1be50a68-e751-4212-ab16-e9f1f1e893c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6057b9a72ec78d1e79357e18cd9a086" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="19d55dec-64db-48ca-8a2a-bb7d318d4195"/>
@@ -3268,10 +3223,78 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <f0b696580dd64673b338b9e7e9df6a44 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f0b696580dd64673b338b9e7e9df6a44>
+    <Project_x002f__x0020_contract_x0020_end_x0020_date xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195" xsi:nil="true"/>
+    <df98972e859c4d8ab2c40b27a56d4e28 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Research ＆ Quality Improvement</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c788aced-109f-432d-9368-116094370ebc</TermId>
+        </TermInfo>
+      </Terms>
+    </df98972e859c4d8ab2c40b27a56d4e28>
+    <i4add73f68bf4b718053652e70d0f6db xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i4add73f68bf4b718053652e70d0f6db>
+    <l85a7ec099b64d7b82fb97f30e826380 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l85a7ec099b64d7b82fb97f30e826380>
+    <ie61b6fb19f94649bf6a41580239b97e xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Audits</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ae63694e-9999-473c-882e-084b09c6631d</TermId>
+        </TermInfo>
+      </Terms>
+    </ie61b6fb19f94649bf6a41580239b97e>
+    <c7239f321a1b424087383680b3e8c036 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c7239f321a1b424087383680b3e8c036>
+    <bf89ef746e92483cbe19fd955e43c70f xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </bf89ef746e92483cbe19fd955e43c70f>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1be50a68-e751-4212-ab16-e9f1f1e893c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389C9BEF-224A-47E4-9595-7EE9C5EC2A41}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C6D9BA-BEB7-47BF-B5E9-921F9ABDC951}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="19d55dec-64db-48ca-8a2a-bb7d318d4195"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="1be50a68-e751-4212-ab16-e9f1f1e893c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3289,21 +3312,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C6D9BA-BEB7-47BF-B5E9-921F9ABDC951}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389C9BEF-224A-47E4-9595-7EE9C5EC2A41}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="19d55dec-64db-48ca-8a2a-bb7d318d4195"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="1be50a68-e751-4212-ab16-e9f1f1e893c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update kpi44 description as per KPI 44-49 Query #288
Signed-off-by: anchit-chandran <anchit97123@gmail.com>
</commit_message>
<xml_diff>
--- a/project/npda/dummy_sheets/kpi-specifications/Calculations_AK_20240621 (1).xlsx
+++ b/project/npda/dummy_sheets/kpi-specifications/Calculations_AK_20240621 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ProgrammingWSL\RCPCH\national-paediatric-diabetes-audit\project\npda\dummy_sheets\kpi-specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFAB901-774C-44E4-8330-97221F1F12FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03546428-BA8D-4213-827B-3A61BE306A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E9E080A3-C8CD-4A00-A462-CC1171CA013C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{E9E080A3-C8CD-4A00-A462-CC1171CA013C}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -747,9 +747,6 @@
     <t>Mean of HbA1c measurements (item 17) within the audit period, excluding measurements taken within 90 days of diagnosis</t>
   </si>
   <si>
-    <t>The mean for each patient is calculated. We then calculate the mean of the means.</t>
-  </si>
-  <si>
     <t>Median HbA1c</t>
   </si>
   <si>
@@ -1130,6 +1127,9 @@
   <si>
     <t>Number of patients with Type 1 diabetes who were diagnosed at least 14 days before the end of the audit period 
 (NOTE: Measure 7 AND diabetes diagnosis date &lt; (AUDIT_END_DATE - 14 days))</t>
+  </si>
+  <si>
+    <t>The median for each patient is calculated. We then calculate the mean of the medians.</t>
   </si>
 </sst>
 </file>
@@ -1862,37 +1862,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A2" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="115.5" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +1905,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -1927,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>17</v>
@@ -1959,7 +1959,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>22</v>
@@ -1976,7 +1976,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>24</v>
@@ -1993,7 +1993,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>26</v>
@@ -2010,7 +2010,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>28</v>
@@ -2027,7 +2027,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>30</v>
@@ -2329,7 +2329,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>52</v>
@@ -2346,10 +2346,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>74</v>
@@ -2378,13 +2378,13 @@
         <v>52</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -2424,13 +2424,13 @@
         <v>77</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>81</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="45.5" x14ac:dyDescent="0.45">
@@ -2461,13 +2461,13 @@
         <v>89</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G34" s="9"/>
     </row>
@@ -2493,7 +2493,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>89</v>
@@ -2527,17 +2527,17 @@
         <v>32.1</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C38" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>165</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.45">
@@ -2545,13 +2545,13 @@
         <v>32.200000000000003</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>169</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>170</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21"/>
@@ -2561,13 +2561,13 @@
         <v>32.299999999999997</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21"/>
@@ -2734,7 +2734,7 @@
         <v>112</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>113</v>
@@ -2743,7 +2743,7 @@
         <v>114</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="105.5" x14ac:dyDescent="0.45">
@@ -2754,7 +2754,7 @@
         <v>115</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>116</v>
@@ -2763,7 +2763,7 @@
         <v>117</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="90.5" x14ac:dyDescent="0.45">
@@ -2774,10 +2774,10 @@
         <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>119</v>
@@ -2809,7 +2809,7 @@
         <v>17</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
@@ -2817,19 +2817,19 @@
         <v>45</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E56" s="10">
         <v>17</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
@@ -2837,19 +2837,19 @@
         <v>46</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="F57" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
@@ -2857,19 +2857,19 @@
         <v>47</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E58" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="45.5" x14ac:dyDescent="0.45">
@@ -2877,13 +2877,13 @@
         <v>48</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E59" s="10">
         <v>39</v>
@@ -2894,16 +2894,16 @@
         <v>49</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E60" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2914,6 +2914,62 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <f0b696580dd64673b338b9e7e9df6a44 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f0b696580dd64673b338b9e7e9df6a44>
+    <Project_x002f__x0020_contract_x0020_end_x0020_date xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195" xsi:nil="true"/>
+    <df98972e859c4d8ab2c40b27a56d4e28 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Research ＆ Quality Improvement</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c788aced-109f-432d-9368-116094370ebc</TermId>
+        </TermInfo>
+      </Terms>
+    </df98972e859c4d8ab2c40b27a56d4e28>
+    <i4add73f68bf4b718053652e70d0f6db xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </i4add73f68bf4b718053652e70d0f6db>
+    <l85a7ec099b64d7b82fb97f30e826380 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l85a7ec099b64d7b82fb97f30e826380>
+    <ie61b6fb19f94649bf6a41580239b97e xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Audits</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ae63694e-9999-473c-882e-084b09c6631d</TermId>
+        </TermInfo>
+      </Terms>
+    </ie61b6fb19f94649bf6a41580239b97e>
+    <c7239f321a1b424087383680b3e8c036 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c7239f321a1b424087383680b3e8c036>
+    <bf89ef746e92483cbe19fd955e43c70f xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </bf89ef746e92483cbe19fd955e43c70f>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1be50a68-e751-4212-ab16-e9f1f1e893c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003773CFE9AFA7D54A9CADE54E78DC4341" ma:contentTypeVersion="31" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="661715b63b6f9491f01d170149810120">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="19d55dec-64db-48ca-8a2a-bb7d318d4195" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="1be50a68-e751-4212-ab16-e9f1f1e893c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6057b9a72ec78d1e79357e18cd9a086" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="19d55dec-64db-48ca-8a2a-bb7d318d4195"/>
@@ -3223,63 +3279,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <f0b696580dd64673b338b9e7e9df6a44 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f0b696580dd64673b338b9e7e9df6a44>
-    <Project_x002f__x0020_contract_x0020_end_x0020_date xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195" xsi:nil="true"/>
-    <df98972e859c4d8ab2c40b27a56d4e28 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Research ＆ Quality Improvement</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c788aced-109f-432d-9368-116094370ebc</TermId>
-        </TermInfo>
-      </Terms>
-    </df98972e859c4d8ab2c40b27a56d4e28>
-    <i4add73f68bf4b718053652e70d0f6db xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </i4add73f68bf4b718053652e70d0f6db>
-    <l85a7ec099b64d7b82fb97f30e826380 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l85a7ec099b64d7b82fb97f30e826380>
-    <ie61b6fb19f94649bf6a41580239b97e xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Audits</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ae63694e-9999-473c-882e-084b09c6631d</TermId>
-        </TermInfo>
-      </Terms>
-    </ie61b6fb19f94649bf6a41580239b97e>
-    <c7239f321a1b424087383680b3e8c036 xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c7239f321a1b424087383680b3e8c036>
-    <bf89ef746e92483cbe19fd955e43c70f xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </bf89ef746e92483cbe19fd955e43c70f>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1be50a68-e751-4212-ab16-e9f1f1e893c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19d55dec-64db-48ca-8a2a-bb7d318d4195">
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389C9BEF-224A-47E4-9595-7EE9C5EC2A41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC62889-5A29-4F3B-8FF5-9B333D0D3FCF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="19d55dec-64db-48ca-8a2a-bb7d318d4195"/>
+    <ds:schemaRef ds:uri="1be50a68-e751-4212-ab16-e9f1f1e893c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C6D9BA-BEB7-47BF-B5E9-921F9ABDC951}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3297,24 +3317,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC62889-5A29-4F3B-8FF5-9B333D0D3FCF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="19d55dec-64db-48ca-8a2a-bb7d318d4195"/>
-    <ds:schemaRef ds:uri="1be50a68-e751-4212-ab16-e9f1f1e893c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389C9BEF-224A-47E4-9595-7EE9C5EC2A41}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>